<commit_message>
Conditional functions + Budget Project update with conditional functions.
</commit_message>
<xml_diff>
--- a/Excel Functions.xlsx
+++ b/Excel Functions.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85F6F28-B220-4427-A5F8-CA6B28548EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5B63C2-9E31-44C5-A4B0-3380C67A0777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{8557D656-55CF-4ABB-9B31-8146A61DE542}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="4" xr2:uid="{8557D656-55CF-4ABB-9B31-8146A61DE542}"/>
   </bookViews>
   <sheets>
     <sheet name="Data used iin Formulas sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Basic Formulas" sheetId="2" r:id="rId2"/>
     <sheet name="The Status Bar" sheetId="3" r:id="rId3"/>
+    <sheet name="Summary Statistics-conditional" sheetId="4" r:id="rId4"/>
+    <sheet name="Dynamica criteria in IFS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,8 +55,26 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={70EE9696-BEE2-4BFE-A2CF-162911379084}</author>
+  </authors>
+  <commentList>
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{70EE9696-BEE2-4BFE-A2CF-162911379084}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Due to less amount of data the combination of Quantity and Flavor only gives 1 number mostly</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>TOTAL VALUE FROM THE OTHER WORKSHEET</t>
   </si>
@@ -141,6 +161,30 @@
   </si>
   <si>
     <t>STD DEV INPUTS</t>
+  </si>
+  <si>
+    <t>COUNTIFS</t>
+  </si>
+  <si>
+    <t>SUMIFS</t>
+  </si>
+  <si>
+    <t>AVERAGEIFS</t>
+  </si>
+  <si>
+    <t>PRICE Sum for all orders with order quantity &gt;3</t>
+  </si>
+  <si>
+    <t>NUM OF SALES</t>
+  </si>
+  <si>
+    <t>SUM TOTAL SALES ($)</t>
+  </si>
+  <si>
+    <t>AVG SALES ($)</t>
+  </si>
+  <si>
+    <t>ORDER QUANTITY THRESHOLDS</t>
   </si>
 </sst>
 </file>
@@ -205,7 +249,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -298,7 +342,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,6 +370,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -656,6 +701,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C16" dT="2022-01-27T20:27:15.90" personId="{524A985A-7271-406C-B6A1-96A697C611E5}" id="{70EE9696-BEE2-4BFE-A2CF-162911379084}">
+    <text>Due to less amount of data the combination of Quantity and Flavor only gives 1 number mostly</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3068B6-588F-45CD-87E2-629DD3E324C8}">
   <dimension ref="A1:H14"/>
@@ -664,7 +717,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +965,7 @@
   <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448DDF51-291D-4CC5-94E7-7FC05E4FD1A2}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,4 +1189,496 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D488DC11-983F-4824-A680-B224272EC928}">
+  <dimension ref="B1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, "snow cream")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, "snow cream")</f>
+        <v>71.58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, "snow cream")</f>
+        <v>23.86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;3")</f>
+        <v>179.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3996E8A9-D36C-48BF-AF68-99D4B8473A6B}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A2)</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A2)</f>
+        <v>19.95</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A2)</f>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A3)</f>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A3)</f>
+        <v>71.58</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A3)</f>
+        <v>23.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A4)</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A4)</f>
+        <v>55.72</v>
+      </c>
+      <c r="D4">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A4)</f>
+        <v>27.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A5)</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A5)</f>
+        <v>20.88</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A5)</f>
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A6)</f>
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A6)</f>
+        <v>63.68</v>
+      </c>
+      <c r="D6">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A6)</f>
+        <v>31.84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <f>COUNTIFS('Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A7)</f>
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!A7)</f>
+        <v>20.9</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D,'Data used iin Formulas sheet'!B:B,'Dynamica criteria in IFS'!A7)</f>
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, "&gt;="&amp;A10)</f>
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A10)</f>
+        <v>252.70999999999998</v>
+      </c>
+      <c r="D10">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A10)</f>
+        <v>25.270999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, "&gt;="&amp;A11)</f>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A11)</f>
+        <v>252.70999999999998</v>
+      </c>
+      <c r="D11">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A11)</f>
+        <v>25.270999999999997</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, "&gt;="&amp;A12)</f>
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A12)</f>
+        <v>220.89</v>
+      </c>
+      <c r="D12">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A12)</f>
+        <v>27.611249999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, "&gt;="&amp;A13)</f>
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A13)</f>
+        <v>179.13</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A13)</f>
+        <v>29.855</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, "&gt;="&amp;A14)</f>
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A14)</f>
+        <v>115.44999999999999</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, "&gt;="&amp;A14)</f>
+        <v>28.862499999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A17, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B17)</f>
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A17, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B17)</f>
+        <v>15.92</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A17, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B17)</f>
+        <v>15.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A18, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B18)</f>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A18, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B18)</f>
+        <v>15.9</v>
+      </c>
+      <c r="E18">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A18, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B18)</f>
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A19, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B19)</f>
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A19, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B19)</f>
+        <v>20.88</v>
+      </c>
+      <c r="E19">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A19, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B19)</f>
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A20, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B20)</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A20, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B20)</f>
+        <v>20.88</v>
+      </c>
+      <c r="E20">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A20, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B20)</f>
+        <v>20.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A21, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B21)</f>
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A21, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B21)</f>
+        <v>63.68</v>
+      </c>
+      <c r="E21">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A21, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B21)</f>
+        <v>31.84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A22, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B22)</f>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A22, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B22)</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E22">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A22, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B22)</f>
+        <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A23, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B23)</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A23, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B23)</f>
+        <v>19.95</v>
+      </c>
+      <c r="E23">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A23, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B23)</f>
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>5</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A24, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B24)</f>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A24, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B24)</f>
+        <v>20.9</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A24, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B24)</f>
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <f>COUNTIFS('Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A25, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B25)</f>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>SUMIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A25, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B25)</f>
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGEIFS('Data used iin Formulas sheet'!D:D, 'Data used iin Formulas sheet'!C:C, 'Dynamica criteria in IFS'!A25, 'Data used iin Formulas sheet'!B:B, 'Dynamica criteria in IFS'!B25)</f>
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:B25">
+    <sortCondition ref="B17:B25"/>
+    <sortCondition ref="A17:A25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Learned date, time features. Budget project: add monthly savings calculator for desired goal.
</commit_message>
<xml_diff>
--- a/Excel Functions.xlsx
+++ b/Excel Functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Desktop\Data Science\ZTM_Excel_Mastery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5B63C2-9E31-44C5-A4B0-3380C67A0777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43BD637-22D3-4CC2-B8AD-A1E34F570EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="1" activeTab="4" xr2:uid="{8557D656-55CF-4ABB-9B31-8146A61DE542}"/>
   </bookViews>
@@ -194,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,12 +244,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">

</xml_diff>